<commit_message>
Updated "Temperature responses.R" in line with manuscript
</commit_message>
<xml_diff>
--- a/Climate data/Climate station data.xlsx
+++ b/Climate data/Climate station data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.johnson/Documents/GitHub/Johnson_Insect_Responses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.johnson/Documents/GitHub/Johnson_Insect_Responses/Climate data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB785AEC-9D13-A446-8E35-48B9D542A960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D01EF0-852B-5046-8B49-F9D6088BEA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28420" yWindow="3820" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="1880" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Climate station data" sheetId="1" r:id="rId1"/>
@@ -176,145 +176,145 @@
     <t>Subtropical</t>
   </si>
   <si>
+    <t>LEEMING</t>
+  </si>
+  <si>
+    <t>UKM00003257</t>
+  </si>
+  <si>
+    <t>Rhopalosiphum rufiabdominalis US Naples</t>
+  </si>
+  <si>
+    <t>NAPLES,_FL</t>
+  </si>
+  <si>
+    <t>USC00086078</t>
+  </si>
+  <si>
+    <t>Aphis nasturtii US Weston</t>
+  </si>
+  <si>
+    <t>FT_LAUDERDALE,_FL</t>
+  </si>
+  <si>
+    <t>USC00083163</t>
+  </si>
+  <si>
+    <t>Eriosoma lanigerum Australia Yathroo</t>
+  </si>
+  <si>
+    <t>WONGAN_HILLS</t>
+  </si>
+  <si>
+    <t>ASN00008137</t>
+  </si>
+  <si>
+    <t>Macrosiphum euphorbiae Canada</t>
+  </si>
+  <si>
+    <t>SARNIA_CLIMATE,_ON</t>
+  </si>
+  <si>
+    <t>CA006127519</t>
+  </si>
+  <si>
+    <t>Myzus persicae Canada</t>
+  </si>
+  <si>
+    <t>CA006127520</t>
+  </si>
+  <si>
+    <t>Hyperomyzus lactucae Australia Acton</t>
+  </si>
+  <si>
+    <t>CANBERRA_AIRPORT_COMPARISON</t>
+  </si>
+  <si>
+    <t>ASN00070014</t>
+  </si>
+  <si>
+    <t>Aphis gossypii China Henan</t>
+  </si>
+  <si>
+    <t>Aulacorthum solani US Ithaca</t>
+  </si>
+  <si>
+    <t>ITHACA_CORNELL_UNIV,_NY</t>
+  </si>
+  <si>
+    <t>USC00304174</t>
+  </si>
+  <si>
+    <t>Brevicoryne brassicae US Columbia</t>
+  </si>
+  <si>
+    <t>COLUMBIA_U_OF_M,_MO</t>
+  </si>
+  <si>
+    <t>USC00231801</t>
+  </si>
+  <si>
+    <t>Myzus persicae US Columbia</t>
+  </si>
+  <si>
+    <t>USC00231802</t>
+  </si>
+  <si>
+    <t>Hyadaphis pseudobrassicae US Columbia</t>
+  </si>
+  <si>
+    <t>USC00231803</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>China Dafeng</t>
+  </si>
+  <si>
+    <t>China Langfang</t>
+  </si>
+  <si>
+    <t>China Xinxiang</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>US Naples</t>
+  </si>
+  <si>
+    <t>US Weston</t>
+  </si>
+  <si>
+    <t>Australia Yathroo</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Australia Acton</t>
+  </si>
+  <si>
+    <t>China Henan</t>
+  </si>
+  <si>
+    <t>US Ithaca</t>
+  </si>
+  <si>
+    <t>US Columbia</t>
+  </si>
+  <si>
+    <t>UK Sand Hutton</t>
+  </si>
+  <si>
     <t>Acyrthosiphon pisum UK Sand Hutton</t>
-  </si>
-  <si>
-    <t>LEEMING</t>
-  </si>
-  <si>
-    <t>UKM00003257</t>
-  </si>
-  <si>
-    <t>Rhopalosiphum rufiabdominalis US Naples</t>
-  </si>
-  <si>
-    <t>NAPLES,_FL</t>
-  </si>
-  <si>
-    <t>USC00086078</t>
-  </si>
-  <si>
-    <t>Aphis nasturtii US Weston</t>
-  </si>
-  <si>
-    <t>FT_LAUDERDALE,_FL</t>
-  </si>
-  <si>
-    <t>USC00083163</t>
-  </si>
-  <si>
-    <t>Eriosoma lanigerum Australia Yathroo</t>
-  </si>
-  <si>
-    <t>WONGAN_HILLS</t>
-  </si>
-  <si>
-    <t>ASN00008137</t>
-  </si>
-  <si>
-    <t>Macrosiphum euphorbiae Canada</t>
-  </si>
-  <si>
-    <t>SARNIA_CLIMATE,_ON</t>
-  </si>
-  <si>
-    <t>CA006127519</t>
-  </si>
-  <si>
-    <t>Myzus persicae Canada</t>
-  </si>
-  <si>
-    <t>CA006127520</t>
-  </si>
-  <si>
-    <t>Hyperomyzus lactucae Australia Acton</t>
-  </si>
-  <si>
-    <t>CANBERRA_AIRPORT_COMPARISON</t>
-  </si>
-  <si>
-    <t>ASN00070014</t>
-  </si>
-  <si>
-    <t>Aphis gossypii China Henan</t>
-  </si>
-  <si>
-    <t>Aulacorthum solani US Ithaca</t>
-  </si>
-  <si>
-    <t>ITHACA_CORNELL_UNIV,_NY</t>
-  </si>
-  <si>
-    <t>USC00304174</t>
-  </si>
-  <si>
-    <t>Brevicoryne brassicae US Columbia</t>
-  </si>
-  <si>
-    <t>COLUMBIA_U_OF_M,_MO</t>
-  </si>
-  <si>
-    <t>USC00231801</t>
-  </si>
-  <si>
-    <t>Myzus persicae US Columbia</t>
-  </si>
-  <si>
-    <t>USC00231802</t>
-  </si>
-  <si>
-    <t>Hyadaphis pseudobrassicae US Columbia</t>
-  </si>
-  <si>
-    <t>USC00231803</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Benin</t>
-  </si>
-  <si>
-    <t>Nigeria</t>
-  </si>
-  <si>
-    <t>China Dafeng</t>
-  </si>
-  <si>
-    <t>China Langfang</t>
-  </si>
-  <si>
-    <t>China Xinxiang</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>UK Sand Hutton</t>
-  </si>
-  <si>
-    <t>US Naples</t>
-  </si>
-  <si>
-    <t>US Weston</t>
-  </si>
-  <si>
-    <t>Australia Yathroo</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>Australia Acton</t>
-  </si>
-  <si>
-    <t>China Henan</t>
-  </si>
-  <si>
-    <t>US Ithaca</t>
-  </si>
-  <si>
-    <t>US Columbia</t>
   </si>
 </sst>
 </file>
@@ -367,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -591,7 +591,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -606,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -662,7 +662,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="1">
         <v>6.45</v>
@@ -719,7 +719,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1">
         <v>6.45</v>
@@ -776,7 +776,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="1">
         <v>7.45</v>
@@ -833,7 +833,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="1">
         <v>33.33</v>
@@ -890,7 +890,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="1">
         <v>33.33</v>
@@ -947,7 +947,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="1">
         <v>39.880000000000003</v>
@@ -1004,7 +1004,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="1">
         <v>35.53</v>
@@ -1061,7 +1061,7 @@
         <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1">
         <v>-21.23</v>
@@ -1118,7 +1118,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="1">
         <v>-21.23</v>
@@ -1175,7 +1175,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1">
         <v>-21.23</v>
@@ -1229,10 +1229,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C12" s="1">
         <v>54.02</v>
@@ -1244,7 +1244,7 @@
         <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="1">
         <v>54.3</v>
@@ -1256,7 +1256,7 @@
         <v>40</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K12" s="1">
         <v>3257</v>
@@ -1286,10 +1286,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C13" s="1">
         <v>26.14</v>
@@ -1301,7 +1301,7 @@
         <v>39</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" s="1">
         <v>26.17</v>
@@ -1313,7 +1313,7 @@
         <v>12</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L13" s="1">
         <v>1942</v>
@@ -1340,10 +1340,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C14" s="1">
         <v>26.14</v>
@@ -1355,7 +1355,7 @@
         <v>39</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" s="1">
         <v>26.1</v>
@@ -1367,7 +1367,7 @@
         <v>5</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L14" s="1">
         <v>1912</v>
@@ -1394,10 +1394,10 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1">
         <v>-30.9</v>
@@ -1409,7 +1409,7 @@
         <v>39</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15" s="1">
         <v>-30.89</v>
@@ -1421,7 +1421,7 @@
         <v>283</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K15" s="1">
         <v>94622</v>
@@ -1451,10 +1451,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1">
         <v>42.81</v>
@@ -1466,7 +1466,7 @@
         <v>39</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G16" s="1">
         <v>43</v>
@@ -1478,7 +1478,7 @@
         <v>181</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K16" s="1">
         <v>71746</v>
@@ -1508,10 +1508,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C17" s="1">
         <v>42.81</v>
@@ -1523,7 +1523,7 @@
         <v>39</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" s="1">
         <v>43</v>
@@ -1535,7 +1535,7 @@
         <v>181</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K17" s="1">
         <v>71746</v>
@@ -1565,10 +1565,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1">
         <v>-35.270000000000003</v>
@@ -1580,7 +1580,7 @@
         <v>39</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G18" s="1">
         <v>-35.299999999999997</v>
@@ -1592,7 +1592,7 @@
         <v>578</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K18" s="1">
         <v>95926</v>
@@ -1622,10 +1622,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1">
         <v>36.07</v>
@@ -1679,10 +1679,10 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C20" s="1">
         <v>42.42</v>
@@ -1694,7 +1694,7 @@
         <v>39</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G20" s="1">
         <v>42.45</v>
@@ -1706,7 +1706,7 @@
         <v>293</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L20" s="1">
         <v>1893</v>
@@ -1733,10 +1733,10 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C21" s="1">
         <v>38.93</v>
@@ -1748,7 +1748,7 @@
         <v>39</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" s="1">
         <v>38.94</v>
@@ -1760,7 +1760,7 @@
         <v>235</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L21" s="1">
         <v>1997</v>
@@ -1787,10 +1787,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C22" s="1">
         <v>38.93</v>
@@ -1802,7 +1802,7 @@
         <v>39</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" s="1">
         <v>38.94</v>
@@ -1814,7 +1814,7 @@
         <v>235</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L22" s="1">
         <v>1997</v>
@@ -1841,10 +1841,10 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" s="1">
         <v>38.93</v>
@@ -1856,7 +1856,7 @@
         <v>39</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G23" s="1">
         <v>38.94</v>
@@ -1868,7 +1868,7 @@
         <v>235</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L23" s="1">
         <v>1997</v>

</xml_diff>

<commit_message>
Updated "Temperature responses.R", "Model TPC analyses.R", and "Statistical analyses.R" in line with manuscript
</commit_message>
<xml_diff>
--- a/Climate data/Climate station data.xlsx
+++ b/Climate data/Climate station data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.johnson/Documents/GitHub/Johnson_Insect_Responses/Climate data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D01EF0-852B-5046-8B49-F9D6088BEA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231D5BFF-4CB8-5C48-97C7-F0B30095A117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3720" yWindow="1880" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
   <si>
     <t>Species</t>
   </si>
@@ -296,9 +296,6 @@
     <t>Australia Yathroo</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>Australia Acton</t>
   </si>
   <si>
@@ -315,6 +312,78 @@
   </si>
   <si>
     <t>Acyrthosiphon pisum UK Sand Hutton</t>
+  </si>
+  <si>
+    <t>Japan Chiba</t>
+  </si>
+  <si>
+    <t>CHIBA</t>
+  </si>
+  <si>
+    <t>JA000047682</t>
+  </si>
+  <si>
+    <t>Aphis citricola Japan Chiba</t>
+  </si>
+  <si>
+    <t>Aphis gossypii Japan Chiba</t>
+  </si>
+  <si>
+    <t>Toxoptera citricidus on Citrus unshui Japan Chiba</t>
+  </si>
+  <si>
+    <t>Toxoptera citricidus on Citrus aurantium Japan Chiba</t>
+  </si>
+  <si>
+    <t>Pilophorus typicus Japan Kochi</t>
+  </si>
+  <si>
+    <t>Lygus lineolaris US Leland</t>
+  </si>
+  <si>
+    <t>US Lubbock</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Aphis gossypii US Lubbock</t>
+  </si>
+  <si>
+    <t>Aphis gossypii Iran</t>
+  </si>
+  <si>
+    <t>Japan Kochi</t>
+  </si>
+  <si>
+    <t>KOCHI</t>
+  </si>
+  <si>
+    <t>JA000047893</t>
+  </si>
+  <si>
+    <t>US Leland</t>
+  </si>
+  <si>
+    <t>STONEVILLE_EXP_STN,_MS</t>
+  </si>
+  <si>
+    <t>USC00228445</t>
+  </si>
+  <si>
+    <t>LUBBOCK,_TX</t>
+  </si>
+  <si>
+    <t>USW00023042</t>
+  </si>
+  <si>
+    <t>TEHRAN-MEHRABAD</t>
+  </si>
+  <si>
+    <t>IR000407540</t>
+  </si>
+  <si>
+    <t>Canada Chatham</t>
   </si>
 </sst>
 </file>
@@ -588,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -601,7 +670,7 @@
     <col min="3" max="27" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -710,11 +779,11 @@
         <v>1</v>
       </c>
       <c r="R2" s="1">
-        <f t="shared" ref="R2:R23" si="0">O2-L2+1</f>
+        <f t="shared" ref="R2:R24" si="0">O2-L2+1</f>
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -771,7 +840,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -828,7 +897,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -885,7 +954,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -942,7 +1011,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -999,7 +1068,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -1056,7 +1125,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -1113,7 +1182,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
@@ -1170,7 +1239,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -1227,12 +1296,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="1">
         <v>54.02</v>
@@ -1284,7 +1353,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1338,7 +1407,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -1392,7 +1461,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
@@ -1449,12 +1518,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C16" s="1">
         <v>42.81</v>
@@ -1506,12 +1575,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C17" s="1">
         <v>42.81</v>
@@ -1563,12 +1632,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="1">
         <v>-35.270000000000003</v>
@@ -1620,12 +1689,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="1">
         <v>36.07</v>
@@ -1677,12 +1746,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" s="1">
         <v>42.42</v>
@@ -1731,12 +1800,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="1">
         <v>38.93</v>
@@ -1785,12 +1854,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" s="1">
         <v>38.93</v>
@@ -1839,12 +1908,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="1">
         <v>38.93</v>
@@ -1891,6 +1960,459 @@
       <c r="R23" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="1">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="1">
+        <v>35.6</v>
+      </c>
+      <c r="H24" s="1">
+        <v>140.1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>19</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K24" s="1">
+        <v>47682</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1967</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1</v>
+      </c>
+      <c r="N24" s="1">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P24" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>1</v>
+      </c>
+      <c r="R24" s="1">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="1">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="1">
+        <v>35.6</v>
+      </c>
+      <c r="H25" s="1">
+        <v>140.1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>19</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K25" s="1">
+        <v>47682</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1967</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+      <c r="N25" s="1">
+        <v>1</v>
+      </c>
+      <c r="O25" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P25" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>1</v>
+      </c>
+      <c r="R25" s="1">
+        <f t="shared" ref="R25:R31" si="1">O25-L25+1</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="1">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="1">
+        <v>35.6</v>
+      </c>
+      <c r="H26" s="1">
+        <v>140.1</v>
+      </c>
+      <c r="I26" s="1">
+        <v>19</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K26" s="1">
+        <v>47682</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1967</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+      <c r="N26" s="1">
+        <v>1</v>
+      </c>
+      <c r="O26" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P26" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>1</v>
+      </c>
+      <c r="R26" s="1">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="1">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="1">
+        <v>35.6</v>
+      </c>
+      <c r="H27" s="1">
+        <v>140.1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>19</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K27" s="1">
+        <v>47682</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1967</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>1</v>
+      </c>
+      <c r="O27" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P27" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>1</v>
+      </c>
+      <c r="R27" s="1">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="1">
+        <v>33.619999999999997</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="1">
+        <v>33.57</v>
+      </c>
+      <c r="H28" s="1">
+        <v>133.35</v>
+      </c>
+      <c r="I28" s="1">
+        <v>5</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K28" s="1">
+        <v>47893</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1951</v>
+      </c>
+      <c r="M28" s="1">
+        <v>1</v>
+      </c>
+      <c r="N28" s="1">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P28" s="1">
+        <v>9</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>30</v>
+      </c>
+      <c r="R28" s="1">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="1">
+        <v>33.42</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" s="1">
+        <v>33.43</v>
+      </c>
+      <c r="H29" s="1">
+        <v>-90.9</v>
+      </c>
+      <c r="I29" s="1">
+        <v>39</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1930</v>
+      </c>
+      <c r="M29" s="1">
+        <v>2</v>
+      </c>
+      <c r="N29" s="1">
+        <v>1</v>
+      </c>
+      <c r="O29" s="1">
+        <v>2019</v>
+      </c>
+      <c r="P29" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>30</v>
+      </c>
+      <c r="R29" s="1">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="1">
+        <v>33.69</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="1">
+        <v>33.65</v>
+      </c>
+      <c r="H30" s="1">
+        <v>-101.81</v>
+      </c>
+      <c r="I30" s="1">
+        <v>993</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K30" s="1">
+        <v>72267</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1947</v>
+      </c>
+      <c r="M30" s="1">
+        <v>1</v>
+      </c>
+      <c r="N30" s="1">
+        <v>1</v>
+      </c>
+      <c r="O30" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P30" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>2</v>
+      </c>
+      <c r="R30" s="1">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="1">
+        <v>35.57</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="1">
+        <v>35.68</v>
+      </c>
+      <c r="H31" s="1">
+        <v>51.32</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1191</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K31" s="1">
+        <v>40754</v>
+      </c>
+      <c r="L31" s="1">
+        <v>1989</v>
+      </c>
+      <c r="M31" s="1">
+        <v>1</v>
+      </c>
+      <c r="N31" s="1">
+        <v>9</v>
+      </c>
+      <c r="O31" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P31" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>1</v>
+      </c>
+      <c r="R31" s="1">
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up extra files that are beyond scope of manuscript
</commit_message>
<xml_diff>
--- a/Climate data/Climate station data.xlsx
+++ b/Climate data/Climate station data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.johnson/Documents/GitHub/Johnson_Insect_Responses/Climate data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231D5BFF-4CB8-5C48-97C7-F0B30095A117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32481D5A-BB51-F34E-A097-4ACDA896CAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="1880" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5420" yWindow="5080" windowWidth="34560" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Climate station data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="90">
   <si>
     <t>Species</t>
   </si>
@@ -104,15 +104,6 @@
     <t>Clavigralla tomentosicollis Benin</t>
   </si>
   <si>
-    <t>Clavigralla tomentosicollis Nigeria</t>
-  </si>
-  <si>
-    <t>Murtala_Muhammed</t>
-  </si>
-  <si>
-    <t>NIM00065201</t>
-  </si>
-  <si>
     <t>Apolygus lucorum China Dafeng</t>
   </si>
   <si>
@@ -200,190 +191,118 @@
     <t>USC00083163</t>
   </si>
   <si>
+    <t>SARNIA_CLIMATE,_ON</t>
+  </si>
+  <si>
+    <t>CA006127519</t>
+  </si>
+  <si>
+    <t>CA006127520</t>
+  </si>
+  <si>
+    <t>Aphis gossypii China Henan</t>
+  </si>
+  <si>
+    <t>Aulacorthum solani US Ithaca</t>
+  </si>
+  <si>
+    <t>ITHACA_CORNELL_UNIV,_NY</t>
+  </si>
+  <si>
+    <t>USC00304174</t>
+  </si>
+  <si>
+    <t>Brevicoryne brassicae US Columbia</t>
+  </si>
+  <si>
+    <t>COLUMBIA_U_OF_M,_MO</t>
+  </si>
+  <si>
+    <t>USC00231801</t>
+  </si>
+  <si>
+    <t>Myzus persicae US Columbia</t>
+  </si>
+  <si>
+    <t>USC00231802</t>
+  </si>
+  <si>
+    <t>Hyadaphis pseudobrassicae US Columbia</t>
+  </si>
+  <si>
+    <t>USC00231803</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>China Dafeng</t>
+  </si>
+  <si>
+    <t>China Langfang</t>
+  </si>
+  <si>
+    <t>China Xinxiang</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>US Naples</t>
+  </si>
+  <si>
+    <t>US Weston</t>
+  </si>
+  <si>
+    <t>China Henan</t>
+  </si>
+  <si>
+    <t>US Ithaca</t>
+  </si>
+  <si>
+    <t>US Columbia</t>
+  </si>
+  <si>
+    <t>UK Sand Hutton</t>
+  </si>
+  <si>
+    <t>Acyrthosiphon pisum UK Sand Hutton</t>
+  </si>
+  <si>
+    <t>Canada Chatham</t>
+  </si>
+  <si>
+    <t>Macrosiphum euphorbiae Canada Chatham</t>
+  </si>
+  <si>
+    <t>Myzus persicae Canada Chatham</t>
+  </si>
+  <si>
+    <t>Clavigralla tomentosicollis Burkina Faso</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Ouagadougou</t>
+  </si>
+  <si>
+    <t>UVM00065503</t>
+  </si>
+  <si>
     <t>Eriosoma lanigerum Australia Yathroo</t>
   </si>
   <si>
+    <t>Australia Yathroo</t>
+  </si>
+  <si>
     <t>WONGAN_HILLS</t>
   </si>
   <si>
     <t>ASN00008137</t>
-  </si>
-  <si>
-    <t>Macrosiphum euphorbiae Canada</t>
-  </si>
-  <si>
-    <t>SARNIA_CLIMATE,_ON</t>
-  </si>
-  <si>
-    <t>CA006127519</t>
-  </si>
-  <si>
-    <t>Myzus persicae Canada</t>
-  </si>
-  <si>
-    <t>CA006127520</t>
-  </si>
-  <si>
-    <t>Hyperomyzus lactucae Australia Acton</t>
-  </si>
-  <si>
-    <t>CANBERRA_AIRPORT_COMPARISON</t>
-  </si>
-  <si>
-    <t>ASN00070014</t>
-  </si>
-  <si>
-    <t>Aphis gossypii China Henan</t>
-  </si>
-  <si>
-    <t>Aulacorthum solani US Ithaca</t>
-  </si>
-  <si>
-    <t>ITHACA_CORNELL_UNIV,_NY</t>
-  </si>
-  <si>
-    <t>USC00304174</t>
-  </si>
-  <si>
-    <t>Brevicoryne brassicae US Columbia</t>
-  </si>
-  <si>
-    <t>COLUMBIA_U_OF_M,_MO</t>
-  </si>
-  <si>
-    <t>USC00231801</t>
-  </si>
-  <si>
-    <t>Myzus persicae US Columbia</t>
-  </si>
-  <si>
-    <t>USC00231802</t>
-  </si>
-  <si>
-    <t>Hyadaphis pseudobrassicae US Columbia</t>
-  </si>
-  <si>
-    <t>USC00231803</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Benin</t>
-  </si>
-  <si>
-    <t>Nigeria</t>
-  </si>
-  <si>
-    <t>China Dafeng</t>
-  </si>
-  <si>
-    <t>China Langfang</t>
-  </si>
-  <si>
-    <t>China Xinxiang</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>US Naples</t>
-  </si>
-  <si>
-    <t>US Weston</t>
-  </si>
-  <si>
-    <t>Australia Yathroo</t>
-  </si>
-  <si>
-    <t>Australia Acton</t>
-  </si>
-  <si>
-    <t>China Henan</t>
-  </si>
-  <si>
-    <t>US Ithaca</t>
-  </si>
-  <si>
-    <t>US Columbia</t>
-  </si>
-  <si>
-    <t>UK Sand Hutton</t>
-  </si>
-  <si>
-    <t>Acyrthosiphon pisum UK Sand Hutton</t>
-  </si>
-  <si>
-    <t>Japan Chiba</t>
-  </si>
-  <si>
-    <t>CHIBA</t>
-  </si>
-  <si>
-    <t>JA000047682</t>
-  </si>
-  <si>
-    <t>Aphis citricola Japan Chiba</t>
-  </si>
-  <si>
-    <t>Aphis gossypii Japan Chiba</t>
-  </si>
-  <si>
-    <t>Toxoptera citricidus on Citrus unshui Japan Chiba</t>
-  </si>
-  <si>
-    <t>Toxoptera citricidus on Citrus aurantium Japan Chiba</t>
-  </si>
-  <si>
-    <t>Pilophorus typicus Japan Kochi</t>
-  </si>
-  <si>
-    <t>Lygus lineolaris US Leland</t>
-  </si>
-  <si>
-    <t>US Lubbock</t>
-  </si>
-  <si>
-    <t>Iran</t>
-  </si>
-  <si>
-    <t>Aphis gossypii US Lubbock</t>
-  </si>
-  <si>
-    <t>Aphis gossypii Iran</t>
-  </si>
-  <si>
-    <t>Japan Kochi</t>
-  </si>
-  <si>
-    <t>KOCHI</t>
-  </si>
-  <si>
-    <t>JA000047893</t>
-  </si>
-  <si>
-    <t>US Leland</t>
-  </si>
-  <si>
-    <t>STONEVILLE_EXP_STN,_MS</t>
-  </si>
-  <si>
-    <t>USC00228445</t>
-  </si>
-  <si>
-    <t>LUBBOCK,_TX</t>
-  </si>
-  <si>
-    <t>USW00023042</t>
-  </si>
-  <si>
-    <t>TEHRAN-MEHRABAD</t>
-  </si>
-  <si>
-    <t>IR000407540</t>
-  </si>
-  <si>
-    <t>Canada Chatham</t>
   </si>
 </sst>
 </file>
@@ -411,7 +330,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -657,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -675,7 +594,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -731,7 +650,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1">
         <v>6.45</v>
@@ -779,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="R2" s="1">
-        <f t="shared" ref="R2:R24" si="0">O2-L2+1</f>
+        <f t="shared" ref="R2:R22" si="0">O2-L2+1</f>
         <v>81</v>
       </c>
     </row>
@@ -788,7 +707,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C3" s="1">
         <v>6.45</v>
@@ -842,13 +761,13 @@
     </row>
     <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1">
-        <v>7.45</v>
+        <v>12.38</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>18</v>
@@ -857,64 +776,64 @@
         <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="G4" s="1">
-        <v>6.58</v>
+        <v>12.35</v>
       </c>
       <c r="H4" s="1">
-        <v>3.32</v>
+        <v>-1.51</v>
       </c>
       <c r="I4" s="1">
-        <v>41</v>
+        <v>316</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="K4" s="1">
-        <v>65201</v>
+        <v>65503</v>
       </c>
       <c r="L4" s="1">
-        <v>1998</v>
+        <v>1973</v>
       </c>
       <c r="M4" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="N4" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O4" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="P4" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="R4" s="1">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1">
         <v>33.33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1">
         <v>32.85</v>
@@ -926,7 +845,7 @@
         <v>5</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K5" s="2">
         <v>58251</v>
@@ -956,22 +875,22 @@
     </row>
     <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C6" s="1">
         <v>33.33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1">
         <v>32.85</v>
@@ -983,7 +902,7 @@
         <v>5</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K6" s="2">
         <v>58251</v>
@@ -1013,22 +932,22 @@
     </row>
     <row r="7" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C7" s="1">
         <v>39.880000000000003</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1">
         <v>39.93</v>
@@ -1040,7 +959,7 @@
         <v>55</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K7" s="1">
         <v>54511</v>
@@ -1070,22 +989,22 @@
     </row>
     <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C8" s="1">
         <v>35.53</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1">
         <v>36.049999999999997</v>
@@ -1097,7 +1016,7 @@
         <v>64</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K8" s="1">
         <v>53898</v>
@@ -1127,10 +1046,10 @@
     </row>
     <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1">
         <v>-21.23</v>
@@ -1139,10 +1058,10 @@
         <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G9" s="1">
         <v>-21.77</v>
@@ -1154,7 +1073,7 @@
         <v>911</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K9" s="1">
         <v>83692</v>
@@ -1184,10 +1103,10 @@
     </row>
     <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1">
         <v>-21.23</v>
@@ -1196,10 +1115,10 @@
         <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G10" s="1">
         <v>-21.77</v>
@@ -1211,7 +1130,7 @@
         <v>911</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K10" s="1">
         <v>83692</v>
@@ -1241,10 +1160,10 @@
     </row>
     <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C11" s="1">
         <v>-21.23</v>
@@ -1253,10 +1172,10 @@
         <v>18</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G11" s="1">
         <v>-21.77</v>
@@ -1268,7 +1187,7 @@
         <v>911</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K11" s="1">
         <v>83692</v>
@@ -1298,22 +1217,22 @@
     </row>
     <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C12" s="1">
         <v>54.02</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G12" s="1">
         <v>54.3</v>
@@ -1325,7 +1244,7 @@
         <v>40</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K12" s="1">
         <v>3257</v>
@@ -1355,22 +1274,22 @@
     </row>
     <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1">
         <v>26.14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G13" s="1">
         <v>26.17</v>
@@ -1382,8 +1301,9 @@
         <v>12</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="K13" s="3"/>
       <c r="L13" s="1">
         <v>1942</v>
       </c>
@@ -1409,22 +1329,22 @@
     </row>
     <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1">
         <v>26.14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G14" s="1">
         <v>26.1</v>
@@ -1436,8 +1356,9 @@
         <v>5</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="K14" s="3"/>
       <c r="L14" s="1">
         <v>1912</v>
       </c>
@@ -1463,79 +1384,79 @@
     </row>
     <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C15" s="1">
-        <v>-30.9</v>
+        <v>42.81</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G15" s="1">
-        <v>-30.89</v>
+        <v>43</v>
       </c>
       <c r="H15" s="1">
-        <v>116.72</v>
+        <v>-82.3</v>
       </c>
       <c r="I15" s="1">
-        <v>283</v>
+        <v>181</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K15" s="1">
-        <v>94622</v>
+        <v>71746</v>
       </c>
       <c r="L15" s="1">
-        <v>1966</v>
+        <v>2006</v>
       </c>
       <c r="M15" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N15" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="O15" s="1">
         <v>2021</v>
       </c>
       <c r="P15" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q15" s="1">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="R15" s="1">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="C16" s="1">
         <v>42.81</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G16" s="1">
         <v>43</v>
@@ -1547,7 +1468,7 @@
         <v>181</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K16" s="1">
         <v>71746</v>
@@ -1575,156 +1496,154 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="C17" s="1">
-        <v>42.81</v>
+        <v>-30.9</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="G17" s="1">
-        <v>43</v>
+        <v>-30.89</v>
       </c>
       <c r="H17" s="1">
-        <v>-82.3</v>
+        <v>116.72</v>
       </c>
       <c r="I17" s="1">
-        <v>181</v>
+        <v>283</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="K17" s="1">
-        <v>71746</v>
+        <v>94622</v>
       </c>
       <c r="L17" s="1">
-        <v>2006</v>
+        <v>1966</v>
       </c>
       <c r="M17" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N17" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="O17" s="1">
         <v>2021</v>
       </c>
       <c r="P17" s="1">
+        <v>9</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>30</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="1">
+        <v>36.07</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="1">
+        <v>36.049999999999997</v>
+      </c>
+      <c r="H18" s="1">
+        <v>114.4</v>
+      </c>
+      <c r="I18" s="1">
+        <v>64</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="1">
+        <v>53898</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1951</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1">
+        <v>1</v>
+      </c>
+      <c r="O18" s="1">
+        <v>2021</v>
+      </c>
+      <c r="P18" s="1">
         <v>10</v>
       </c>
-      <c r="Q17" s="1">
-        <v>2</v>
-      </c>
-      <c r="R17" s="1">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="1">
-        <v>-35.270000000000003</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="1">
-        <v>-35.299999999999997</v>
-      </c>
-      <c r="H18" s="1">
-        <v>149.19999999999999</v>
-      </c>
-      <c r="I18" s="1">
-        <v>578</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K18" s="1">
-        <v>95926</v>
-      </c>
-      <c r="L18" s="1">
-        <v>1939</v>
-      </c>
-      <c r="M18" s="1">
-        <v>3</v>
-      </c>
-      <c r="N18" s="1">
-        <v>1</v>
-      </c>
-      <c r="O18" s="1">
-        <v>2010</v>
-      </c>
-      <c r="P18" s="1">
-        <v>12</v>
-      </c>
       <c r="Q18" s="1">
         <v>1</v>
       </c>
       <c r="R18" s="1">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>66</v>
+      <c r="A19" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1">
-        <v>36.07</v>
+        <v>42.42</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="G19" s="1">
-        <v>36.049999999999997</v>
+        <v>42.45</v>
       </c>
       <c r="H19" s="1">
-        <v>114.4</v>
+        <v>-76.45</v>
       </c>
       <c r="I19" s="1">
-        <v>64</v>
+        <v>293</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K19" s="1">
-        <v>53898</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="K19" s="3"/>
       <c r="L19" s="1">
-        <v>1951</v>
+        <v>1893</v>
       </c>
       <c r="M19" s="1">
         <v>1</v>
@@ -1743,48 +1662,49 @@
       </c>
       <c r="R19" s="1">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>67</v>
+      <c r="A20" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C20" s="1">
-        <v>42.42</v>
+        <v>38.93</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G20" s="1">
-        <v>42.45</v>
+        <v>38.94</v>
       </c>
       <c r="H20" s="1">
-        <v>-76.45</v>
+        <v>-92.32</v>
       </c>
       <c r="I20" s="1">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="K20" s="3"/>
       <c r="L20" s="1">
-        <v>1893</v>
+        <v>1997</v>
       </c>
       <c r="M20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N20" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="O20" s="1">
         <v>2021</v>
@@ -1797,27 +1717,27 @@
       </c>
       <c r="R20" s="1">
         <f t="shared" si="0"/>
-        <v>129</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>70</v>
+      <c r="A21" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1">
         <v>38.93</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="G21" s="1">
         <v>38.94</v>
@@ -1829,8 +1749,9 @@
         <v>235</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="K21" s="3"/>
       <c r="L21" s="1">
         <v>1997</v>
       </c>
@@ -1855,23 +1776,23 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>73</v>
+      <c r="A22" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C22" s="1">
         <v>38.93</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="G22" s="1">
         <v>38.94</v>
@@ -1883,8 +1804,9 @@
         <v>235</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="K22" s="3"/>
       <c r="L22" s="1">
         <v>1997</v>
       </c>
@@ -1906,513 +1828,6 @@
       <c r="R22" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="1">
-        <v>38.93</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="1">
-        <v>38.94</v>
-      </c>
-      <c r="H23" s="1">
-        <v>-92.32</v>
-      </c>
-      <c r="I23" s="1">
-        <v>235</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L23" s="1">
-        <v>1997</v>
-      </c>
-      <c r="M23" s="1">
-        <v>2</v>
-      </c>
-      <c r="N23" s="1">
-        <v>14</v>
-      </c>
-      <c r="O23" s="1">
-        <v>2021</v>
-      </c>
-      <c r="P23" s="1">
-        <v>10</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>1</v>
-      </c>
-      <c r="R23" s="1">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="1">
-        <v>35.380000000000003</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G24" s="1">
-        <v>35.6</v>
-      </c>
-      <c r="H24" s="1">
-        <v>140.1</v>
-      </c>
-      <c r="I24" s="1">
-        <v>19</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K24" s="1">
-        <v>47682</v>
-      </c>
-      <c r="L24" s="1">
-        <v>1967</v>
-      </c>
-      <c r="M24" s="1">
-        <v>1</v>
-      </c>
-      <c r="N24" s="1">
-        <v>1</v>
-      </c>
-      <c r="O24" s="1">
-        <v>2021</v>
-      </c>
-      <c r="P24" s="1">
-        <v>10</v>
-      </c>
-      <c r="Q24" s="1">
-        <v>1</v>
-      </c>
-      <c r="R24" s="1">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="1">
-        <v>35.380000000000003</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="1">
-        <v>35.6</v>
-      </c>
-      <c r="H25" s="1">
-        <v>140.1</v>
-      </c>
-      <c r="I25" s="1">
-        <v>19</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K25" s="1">
-        <v>47682</v>
-      </c>
-      <c r="L25" s="1">
-        <v>1967</v>
-      </c>
-      <c r="M25" s="1">
-        <v>1</v>
-      </c>
-      <c r="N25" s="1">
-        <v>1</v>
-      </c>
-      <c r="O25" s="1">
-        <v>2021</v>
-      </c>
-      <c r="P25" s="1">
-        <v>10</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>1</v>
-      </c>
-      <c r="R25" s="1">
-        <f t="shared" ref="R25:R31" si="1">O25-L25+1</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C26" s="1">
-        <v>35.380000000000003</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" s="1">
-        <v>35.6</v>
-      </c>
-      <c r="H26" s="1">
-        <v>140.1</v>
-      </c>
-      <c r="I26" s="1">
-        <v>19</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K26" s="1">
-        <v>47682</v>
-      </c>
-      <c r="L26" s="1">
-        <v>1967</v>
-      </c>
-      <c r="M26" s="1">
-        <v>1</v>
-      </c>
-      <c r="N26" s="1">
-        <v>1</v>
-      </c>
-      <c r="O26" s="1">
-        <v>2021</v>
-      </c>
-      <c r="P26" s="1">
-        <v>10</v>
-      </c>
-      <c r="Q26" s="1">
-        <v>1</v>
-      </c>
-      <c r="R26" s="1">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="1">
-        <v>35.380000000000003</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="1">
-        <v>35.6</v>
-      </c>
-      <c r="H27" s="1">
-        <v>140.1</v>
-      </c>
-      <c r="I27" s="1">
-        <v>19</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K27" s="1">
-        <v>47682</v>
-      </c>
-      <c r="L27" s="1">
-        <v>1967</v>
-      </c>
-      <c r="M27" s="1">
-        <v>1</v>
-      </c>
-      <c r="N27" s="1">
-        <v>1</v>
-      </c>
-      <c r="O27" s="1">
-        <v>2021</v>
-      </c>
-      <c r="P27" s="1">
-        <v>10</v>
-      </c>
-      <c r="Q27" s="1">
-        <v>1</v>
-      </c>
-      <c r="R27" s="1">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" s="1">
-        <v>33.619999999999997</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G28" s="1">
-        <v>33.57</v>
-      </c>
-      <c r="H28" s="1">
-        <v>133.35</v>
-      </c>
-      <c r="I28" s="1">
-        <v>5</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K28" s="1">
-        <v>47893</v>
-      </c>
-      <c r="L28" s="1">
-        <v>1951</v>
-      </c>
-      <c r="M28" s="1">
-        <v>1</v>
-      </c>
-      <c r="N28" s="1">
-        <v>1</v>
-      </c>
-      <c r="O28" s="1">
-        <v>2021</v>
-      </c>
-      <c r="P28" s="1">
-        <v>9</v>
-      </c>
-      <c r="Q28" s="1">
-        <v>30</v>
-      </c>
-      <c r="R28" s="1">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="1">
-        <v>33.42</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G29" s="1">
-        <v>33.43</v>
-      </c>
-      <c r="H29" s="1">
-        <v>-90.9</v>
-      </c>
-      <c r="I29" s="1">
-        <v>39</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="L29" s="1">
-        <v>1930</v>
-      </c>
-      <c r="M29" s="1">
-        <v>2</v>
-      </c>
-      <c r="N29" s="1">
-        <v>1</v>
-      </c>
-      <c r="O29" s="1">
-        <v>2019</v>
-      </c>
-      <c r="P29" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q29" s="1">
-        <v>30</v>
-      </c>
-      <c r="R29" s="1">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="1">
-        <v>33.69</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="1">
-        <v>33.65</v>
-      </c>
-      <c r="H30" s="1">
-        <v>-101.81</v>
-      </c>
-      <c r="I30" s="1">
-        <v>993</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K30" s="1">
-        <v>72267</v>
-      </c>
-      <c r="L30" s="1">
-        <v>1947</v>
-      </c>
-      <c r="M30" s="1">
-        <v>1</v>
-      </c>
-      <c r="N30" s="1">
-        <v>1</v>
-      </c>
-      <c r="O30" s="1">
-        <v>2021</v>
-      </c>
-      <c r="P30" s="1">
-        <v>10</v>
-      </c>
-      <c r="Q30" s="1">
-        <v>2</v>
-      </c>
-      <c r="R30" s="1">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" s="1">
-        <v>35.57</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31" s="1">
-        <v>35.68</v>
-      </c>
-      <c r="H31" s="1">
-        <v>51.32</v>
-      </c>
-      <c r="I31" s="1">
-        <v>1191</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K31" s="1">
-        <v>40754</v>
-      </c>
-      <c r="L31" s="1">
-        <v>1989</v>
-      </c>
-      <c r="M31" s="1">
-        <v>1</v>
-      </c>
-      <c r="N31" s="1">
-        <v>9</v>
-      </c>
-      <c r="O31" s="1">
-        <v>2021</v>
-      </c>
-      <c r="P31" s="1">
-        <v>10</v>
-      </c>
-      <c r="Q31" s="1">
-        <v>1</v>
-      </c>
-      <c r="R31" s="1">
-        <f t="shared" si="1"/>
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>